<commit_message>
connection with sheet and variable clean up)
</commit_message>
<xml_diff>
--- a/REFrameworkTest/Data/Config.xlsx
+++ b/REFrameworkTest/Data/Config.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -177,13 +177,37 @@
   </si>
   <si>
     <t>The wesite address</t>
+  </si>
+  <si>
+    <t>sheetID</t>
+  </si>
+  <si>
+    <t>keyPath</t>
+  </si>
+  <si>
+    <t>pass</t>
+  </si>
+  <si>
+    <t>serviceAccount</t>
+  </si>
+  <si>
+    <t>15cuHoJGctReyA0OfUClW7AmBeMT2pOD_Qx2clYS9JSY</t>
+  </si>
+  <si>
+    <t>notasecret</t>
+  </si>
+  <si>
+    <t>gsheet@cp100-199412.iam.gserviceaccount.com</t>
+  </si>
+  <si>
+    <t>.\Data\gsheet.p12</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -193,6 +217,12 @@
       <b/>
       <sz val="14"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -213,14 +243,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -501,8 +534,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z997"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -581,10 +614,38 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
     <row r="10" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="11" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1574,6 +1635,9 @@
     <row r="996" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="997" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B9" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>